<commit_message>
Added soft assert validation in TC_LoginExcel_002.
</commit_message>
<xml_diff>
--- a/Guru_Bank/datafiles/loginData.xlsx
+++ b/Guru_Bank/datafiles/loginData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmitSen\eclipse-workspace\Guru_Bank\datafiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmitSen\git\E2E_Selenium_Projects\Guru_Bank\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFA6912-C631-40DE-912F-75E2AEB9E0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7C07EC-ADB9-4140-8EA7-721A6B203E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>UserID</t>
   </si>
@@ -42,7 +42,16 @@
     <t>failed</t>
   </si>
   <si>
+    <t>dypYhev</t>
+  </si>
+  <si>
+    <t>mngr384654</t>
+  </si>
+  <si>
     <t>Passed - Valid Login</t>
+  </si>
+  <si>
+    <t>Failed - Invalid Login</t>
   </si>
 </sst>
 </file>
@@ -361,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,13 +395,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>